<commit_message>
#SSW-1990 update Standard Importe
</commit_message>
<xml_diff>
--- a/Common/Style/Resource/Template/Import_Interessent.xlsx
+++ b/Common/Style/Resource/Template/Import_Interessent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\abteilung_software\Projekte\Schulsoftware\30 Projektrealisierung\30.2 Einstieg und Schulung\!Datenimport\Datenimport feste Spalten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\kundwzwickau.de\kuw\abteilung_software\Projekte\Schulsoftware\30 Projektrealisierung\30.2 Einstieg und Schulung\!Datenimport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70DFD08-BB20-4EB3-AD22-BE8156016D91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D38F22-A3B0-4A79-8DFD-EAB040BACB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kl. 1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="410">
   <si>
     <t>Nr</t>
   </si>
@@ -1488,6 +1488,9 @@
   </si>
   <si>
     <t>08056</t>
+  </si>
+  <si>
+    <t>01.01.2020</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1695,72 +1698,42 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -5501,691 +5474,520 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="31" customWidth="1"/>
-    <col min="11" max="11" width="6" style="32" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="31" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="11.5703125" style="31"/>
-    <col min="33" max="33" width="20.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.5703125" style="32"/>
-    <col min="35" max="43" width="11.5703125" style="31"/>
-    <col min="44" max="44" width="20.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.5703125" style="32"/>
-    <col min="46" max="16384" width="11.5703125" style="31"/>
+    <col min="1" max="1" width="3.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="29" customWidth="1"/>
+    <col min="11" max="11" width="6" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="11.5703125" style="29"/>
+    <col min="33" max="33" width="20.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="34" max="43" width="11.5703125" style="29"/>
+    <col min="44" max="44" width="20.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="11.5703125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="1:50" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35"/>
+      <c r="B1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="30" t="s">
         <v>367</v>
       </c>
-      <c r="G1" s="35">
+      <c r="G1" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>358</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>370</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>371</v>
+      </c>
+      <c r="O1" s="30">
+        <v>7</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>359</v>
+      </c>
+      <c r="S1" s="31">
         <v>43831</v>
       </c>
-      <c r="H1" s="34" t="s">
-        <v>368</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>358</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>407</v>
-      </c>
-      <c r="K1" s="36" t="s">
+      <c r="T1" s="31">
+        <v>43831</v>
+      </c>
+      <c r="U1" s="31">
+        <v>43831</v>
+      </c>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31" t="s">
+        <v>360</v>
+      </c>
+      <c r="X1" s="30" t="s">
+        <v>372</v>
+      </c>
+      <c r="Y1" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="Z1" s="30" t="s">
+        <v>372</v>
+      </c>
+      <c r="AA1" s="30" t="s">
+        <v>374</v>
+      </c>
+      <c r="AB1" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="AC1" s="30" t="s">
+        <v>376</v>
+      </c>
+      <c r="AD1" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="AE1" s="30" t="s">
+        <v>378</v>
+      </c>
+      <c r="AF1" s="30" t="s">
+        <v>365</v>
+      </c>
+      <c r="AG1" s="31" t="s">
+        <v>403</v>
+      </c>
+      <c r="AH1" s="30" t="s">
         <v>408</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="AI1" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="AJ1" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="AK1" s="30" t="s">
         <v>371</v>
       </c>
-      <c r="O1" s="34">
+      <c r="AL1" s="30">
         <v>7</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="AM1" s="30" t="s">
         <v>379</v>
       </c>
-      <c r="Q1" s="37" t="s">
-        <v>311</v>
-      </c>
-      <c r="R1" s="38" t="s">
-        <v>359</v>
-      </c>
-      <c r="S1" s="39">
-        <v>43831</v>
-      </c>
-      <c r="T1" s="39">
-        <v>43831</v>
-      </c>
-      <c r="U1" s="39">
-        <v>43831</v>
-      </c>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37" t="s">
-        <v>360</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>372</v>
-      </c>
-      <c r="Y1" s="34" t="s">
-        <v>373</v>
-      </c>
-      <c r="Z1" s="34" t="s">
-        <v>372</v>
-      </c>
-      <c r="AA1" s="34" t="s">
-        <v>374</v>
-      </c>
-      <c r="AB1" s="40" t="s">
-        <v>375</v>
-      </c>
-      <c r="AC1" s="34" t="s">
-        <v>376</v>
-      </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AN1" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="AO1" s="30" t="s">
         <v>377</v>
       </c>
-      <c r="AE1" s="34" t="s">
-        <v>378</v>
-      </c>
-      <c r="AF1" s="34" t="s">
+      <c r="AP1" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="AQ1" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="AG1" s="37" t="s">
+      <c r="AR1" s="31" t="s">
         <v>403</v>
       </c>
-      <c r="AH1" s="36" t="s">
+      <c r="AS1" s="30" t="s">
         <v>408</v>
       </c>
-      <c r="AI1" s="34" t="s">
+      <c r="AT1" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="AJ1" s="34" t="s">
+      <c r="AU1" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="AK1" s="34" t="s">
+      <c r="AV1" s="30" t="s">
         <v>371</v>
       </c>
-      <c r="AL1" s="34">
+      <c r="AW1" s="30">
         <v>7</v>
       </c>
-      <c r="AM1" s="34" t="s">
+      <c r="AX1" s="30" t="s">
         <v>379</v>
       </c>
-      <c r="AN1" s="34" t="s">
-        <v>380</v>
-      </c>
-      <c r="AO1" s="34" t="s">
-        <v>377</v>
-      </c>
-      <c r="AP1" s="34" t="s">
-        <v>381</v>
-      </c>
-      <c r="AQ1" s="34" t="s">
-        <v>365</v>
-      </c>
-      <c r="AR1" s="37" t="s">
-        <v>403</v>
-      </c>
-      <c r="AS1" s="36" t="s">
-        <v>408</v>
-      </c>
-      <c r="AT1" s="34" t="s">
-        <v>369</v>
-      </c>
-      <c r="AU1" s="34" t="s">
-        <v>370</v>
-      </c>
-      <c r="AV1" s="34" t="s">
-        <v>371</v>
-      </c>
-      <c r="AW1" s="34">
+    </row>
+    <row r="2" spans="1:50" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>350</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>351</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="AX1" s="34" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>363</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>350</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>351</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>406</v>
-      </c>
-      <c r="K2" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="P2" s="32" t="s">
         <v>402</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="Q2" s="32" t="s">
         <v>357</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="R2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="41" t="s">
+      <c r="S2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="T2" s="41" t="s">
+      <c r="T2" s="32" t="s">
         <v>361</v>
       </c>
-      <c r="U2" s="41" t="s">
+      <c r="U2" s="32" t="s">
         <v>362</v>
       </c>
-      <c r="V2" s="41" t="s">
+      <c r="V2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="41" t="s">
+      <c r="W2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="41" t="s">
+      <c r="X2" s="32" t="s">
         <v>352</v>
       </c>
-      <c r="Y2" s="41" t="s">
+      <c r="Y2" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="Z2" s="41" t="s">
+      <c r="Z2" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="AA2" s="41" t="s">
+      <c r="AA2" s="32" t="s">
         <v>355</v>
       </c>
-      <c r="AB2" s="41" t="s">
+      <c r="AB2" s="32" t="s">
         <v>356</v>
       </c>
-      <c r="AC2" s="43" t="s">
+      <c r="AC2" s="33" t="s">
         <v>382</v>
       </c>
-      <c r="AD2" s="43" t="s">
+      <c r="AD2" s="33" t="s">
         <v>383</v>
       </c>
-      <c r="AE2" s="43" t="s">
+      <c r="AE2" s="33" t="s">
         <v>384</v>
       </c>
-      <c r="AF2" s="43" t="s">
+      <c r="AF2" s="33" t="s">
         <v>385</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="AH2" s="45" t="s">
+      <c r="AH2" s="33" t="s">
         <v>386</v>
       </c>
-      <c r="AI2" s="43" t="s">
+      <c r="AI2" s="33" t="s">
         <v>387</v>
       </c>
-      <c r="AJ2" s="43" t="s">
+      <c r="AJ2" s="33" t="s">
         <v>388</v>
       </c>
-      <c r="AK2" s="43" t="s">
+      <c r="AK2" s="33" t="s">
         <v>389</v>
       </c>
-      <c r="AL2" s="43" t="s">
+      <c r="AL2" s="33" t="s">
         <v>390</v>
       </c>
-      <c r="AM2" s="43" t="s">
+      <c r="AM2" s="33" t="s">
         <v>391</v>
       </c>
-      <c r="AN2" s="46" t="s">
+      <c r="AN2" s="34" t="s">
         <v>392</v>
       </c>
-      <c r="AO2" s="46" t="s">
+      <c r="AO2" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="AP2" s="46" t="s">
+      <c r="AP2" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="AQ2" s="46" t="s">
+      <c r="AQ2" s="34" t="s">
         <v>395</v>
       </c>
-      <c r="AR2" s="47" t="s">
+      <c r="AR2" s="39" t="s">
         <v>404</v>
       </c>
-      <c r="AS2" s="48" t="s">
+      <c r="AS2" s="34" t="s">
         <v>396</v>
       </c>
-      <c r="AT2" s="46" t="s">
+      <c r="AT2" s="34" t="s">
         <v>397</v>
       </c>
-      <c r="AU2" s="46" t="s">
+      <c r="AU2" s="34" t="s">
         <v>398</v>
       </c>
-      <c r="AV2" s="46" t="s">
+      <c r="AV2" s="34" t="s">
         <v>399</v>
       </c>
-      <c r="AW2" s="46" t="s">
+      <c r="AW2" s="34" t="s">
         <v>400</v>
       </c>
-      <c r="AX2" s="46" t="s">
+      <c r="AX2" s="34" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="29"/>
-      <c r="K3" s="30"/>
-      <c r="AG3" s="31"/>
-      <c r="AH3" s="30"/>
-      <c r="AR3" s="31"/>
-      <c r="AS3" s="30"/>
+      <c r="AG3" s="29"/>
+      <c r="AR3" s="29"/>
     </row>
     <row r="4" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G4" s="29"/>
-      <c r="K4" s="30"/>
-      <c r="AG4" s="31"/>
-      <c r="AH4" s="30"/>
-      <c r="AR4" s="31"/>
-      <c r="AS4" s="30"/>
+      <c r="AG4" s="29"/>
+      <c r="AR4" s="29"/>
     </row>
     <row r="5" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="29"/>
-      <c r="K5" s="30"/>
-      <c r="AG5" s="31"/>
-      <c r="AH5" s="30"/>
-      <c r="AR5" s="31"/>
-      <c r="AS5" s="30"/>
+      <c r="AG5" s="29"/>
+      <c r="AR5" s="29"/>
     </row>
     <row r="6" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="29"/>
-      <c r="K6" s="30"/>
-      <c r="AG6" s="31"/>
-      <c r="AH6" s="30"/>
-      <c r="AR6" s="31"/>
-      <c r="AS6" s="30"/>
+      <c r="AG6" s="29"/>
+      <c r="AR6" s="29"/>
     </row>
     <row r="7" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="AG7" s="31"/>
-      <c r="AH7" s="30"/>
-      <c r="AR7" s="31"/>
-      <c r="AS7" s="30"/>
+      <c r="AG7" s="29"/>
+      <c r="AR7" s="29"/>
     </row>
     <row r="8" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="29"/>
-      <c r="K8" s="30"/>
-      <c r="AG8" s="31"/>
-      <c r="AH8" s="30"/>
-      <c r="AR8" s="31"/>
-      <c r="AS8" s="30"/>
+      <c r="AG8" s="29"/>
+      <c r="AR8" s="29"/>
     </row>
     <row r="9" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="29"/>
-      <c r="K9" s="30"/>
-      <c r="AG9" s="31"/>
-      <c r="AH9" s="30"/>
-      <c r="AR9" s="31"/>
-      <c r="AS9" s="30"/>
+      <c r="AG9" s="29"/>
+      <c r="AR9" s="29"/>
     </row>
     <row r="10" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G10" s="29"/>
-      <c r="K10" s="30"/>
-      <c r="AG10" s="31"/>
-      <c r="AH10" s="30"/>
-      <c r="AR10" s="31"/>
-      <c r="AS10" s="30"/>
+      <c r="AG10" s="29"/>
+      <c r="AR10" s="29"/>
     </row>
     <row r="11" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G11" s="29"/>
-      <c r="K11" s="30"/>
-      <c r="AG11" s="31"/>
-      <c r="AH11" s="30"/>
-      <c r="AR11" s="31"/>
-      <c r="AS11" s="30"/>
+      <c r="AG11" s="29"/>
+      <c r="AR11" s="29"/>
     </row>
     <row r="12" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G12" s="29"/>
-      <c r="K12" s="30"/>
-      <c r="AG12" s="31"/>
-      <c r="AH12" s="30"/>
-      <c r="AR12" s="31"/>
-      <c r="AS12" s="30"/>
+      <c r="AG12" s="29"/>
+      <c r="AR12" s="29"/>
     </row>
     <row r="13" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="29"/>
-      <c r="K13" s="30"/>
-      <c r="AG13" s="31"/>
-      <c r="AH13" s="30"/>
-      <c r="AR13" s="31"/>
-      <c r="AS13" s="30"/>
+      <c r="AG13" s="29"/>
+      <c r="AR13" s="29"/>
     </row>
     <row r="14" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="29"/>
-      <c r="K14" s="30"/>
-      <c r="AG14" s="31"/>
-      <c r="AH14" s="30"/>
-      <c r="AR14" s="31"/>
-      <c r="AS14" s="30"/>
+      <c r="AG14" s="29"/>
+      <c r="AR14" s="29"/>
     </row>
     <row r="15" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G15" s="29"/>
-      <c r="K15" s="30"/>
-      <c r="AG15" s="31"/>
-      <c r="AH15" s="30"/>
-      <c r="AR15" s="31"/>
-      <c r="AS15" s="30"/>
+      <c r="AG15" s="29"/>
+      <c r="AR15" s="29"/>
     </row>
     <row r="16" spans="1:50" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="29"/>
-      <c r="K16" s="30"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="30"/>
-      <c r="AR16" s="31"/>
-      <c r="AS16" s="30"/>
-    </row>
-    <row r="17" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G17" s="29"/>
-      <c r="K17" s="30"/>
-      <c r="AG17" s="31"/>
-      <c r="AH17" s="30"/>
-      <c r="AR17" s="31"/>
-      <c r="AS17" s="30"/>
-    </row>
-    <row r="18" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G18" s="29"/>
-      <c r="K18" s="30"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="30"/>
-      <c r="AR18" s="31"/>
-      <c r="AS18" s="30"/>
-    </row>
-    <row r="19" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G19" s="29"/>
-      <c r="K19" s="30"/>
-      <c r="AG19" s="31"/>
-      <c r="AH19" s="30"/>
-      <c r="AR19" s="31"/>
-      <c r="AS19" s="30"/>
-    </row>
-    <row r="20" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G20" s="29"/>
-      <c r="K20" s="30"/>
-      <c r="AG20" s="31"/>
-      <c r="AH20" s="30"/>
-      <c r="AR20" s="31"/>
-      <c r="AS20" s="30"/>
-    </row>
-    <row r="21" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="29"/>
-      <c r="K21" s="30"/>
-      <c r="AG21" s="31"/>
-      <c r="AH21" s="30"/>
-      <c r="AR21" s="31"/>
-      <c r="AS21" s="30"/>
-    </row>
-    <row r="22" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="29"/>
-      <c r="K22" s="30"/>
-      <c r="AG22" s="31"/>
-      <c r="AH22" s="30"/>
-      <c r="AR22" s="31"/>
-      <c r="AS22" s="30"/>
-    </row>
-    <row r="23" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G23" s="29"/>
-      <c r="K23" s="30"/>
-      <c r="AG23" s="31"/>
-      <c r="AH23" s="30"/>
-      <c r="AR23" s="31"/>
-      <c r="AS23" s="30"/>
-    </row>
-    <row r="24" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G24" s="29"/>
-      <c r="K24" s="30"/>
-      <c r="AG24" s="31"/>
-      <c r="AH24" s="30"/>
-      <c r="AR24" s="31"/>
-      <c r="AS24" s="30"/>
-    </row>
-    <row r="25" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="29"/>
-      <c r="K25" s="30"/>
-      <c r="AG25" s="31"/>
-      <c r="AH25" s="30"/>
-      <c r="AR25" s="31"/>
-      <c r="AS25" s="30"/>
-    </row>
-    <row r="26" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G26" s="29"/>
-      <c r="K26" s="30"/>
-      <c r="AG26" s="31"/>
-      <c r="AH26" s="30"/>
-      <c r="AR26" s="31"/>
-      <c r="AS26" s="30"/>
-    </row>
-    <row r="27" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="29"/>
-      <c r="K27" s="30"/>
-      <c r="AG27" s="31"/>
-      <c r="AH27" s="30"/>
-      <c r="AR27" s="31"/>
-      <c r="AS27" s="30"/>
-    </row>
-    <row r="28" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G28" s="29"/>
-      <c r="K28" s="30"/>
-      <c r="AG28" s="31"/>
-      <c r="AH28" s="30"/>
-      <c r="AR28" s="31"/>
-      <c r="AS28" s="30"/>
-    </row>
-    <row r="29" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G29" s="29"/>
-      <c r="K29" s="30"/>
-      <c r="AG29" s="31"/>
-      <c r="AH29" s="30"/>
-      <c r="AR29" s="31"/>
-      <c r="AS29" s="30"/>
-    </row>
-    <row r="30" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="29"/>
-      <c r="K30" s="30"/>
-      <c r="AG30" s="31"/>
-      <c r="AH30" s="30"/>
-      <c r="AR30" s="31"/>
-      <c r="AS30" s="30"/>
-    </row>
-    <row r="31" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G31" s="29"/>
-      <c r="K31" s="30"/>
-      <c r="AG31" s="31"/>
-      <c r="AH31" s="30"/>
-      <c r="AR31" s="31"/>
-      <c r="AS31" s="30"/>
-    </row>
-    <row r="32" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G32" s="29"/>
-      <c r="K32" s="30"/>
-      <c r="AG32" s="31"/>
-      <c r="AH32" s="30"/>
-      <c r="AR32" s="31"/>
-      <c r="AS32" s="30"/>
-    </row>
-    <row r="33" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="29"/>
-      <c r="K33" s="30"/>
-      <c r="AG33" s="31"/>
-      <c r="AH33" s="30"/>
-      <c r="AR33" s="31"/>
-      <c r="AS33" s="30"/>
-    </row>
-    <row r="34" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G34" s="29"/>
-      <c r="K34" s="30"/>
-      <c r="AG34" s="31"/>
-      <c r="AH34" s="30"/>
-      <c r="AR34" s="31"/>
-      <c r="AS34" s="30"/>
-    </row>
-    <row r="35" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G35" s="29"/>
-      <c r="K35" s="30"/>
-      <c r="AG35" s="31"/>
-      <c r="AH35" s="30"/>
-      <c r="AR35" s="31"/>
-      <c r="AS35" s="30"/>
-    </row>
-    <row r="36" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G36" s="29"/>
-      <c r="K36" s="30"/>
-      <c r="AG36" s="31"/>
-      <c r="AH36" s="30"/>
-      <c r="AR36" s="31"/>
-      <c r="AS36" s="30"/>
-    </row>
-    <row r="37" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G37" s="29"/>
-      <c r="K37" s="30"/>
-      <c r="AG37" s="31"/>
-      <c r="AH37" s="30"/>
-      <c r="AR37" s="31"/>
-      <c r="AS37" s="30"/>
-    </row>
-    <row r="38" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G38" s="29"/>
-      <c r="K38" s="30"/>
-      <c r="AG38" s="31"/>
-      <c r="AH38" s="30"/>
-      <c r="AR38" s="31"/>
-      <c r="AS38" s="30"/>
-    </row>
-    <row r="39" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G39" s="29"/>
-      <c r="K39" s="30"/>
-      <c r="AG39" s="31"/>
-      <c r="AH39" s="30"/>
-      <c r="AR39" s="31"/>
-      <c r="AS39" s="30"/>
-    </row>
-    <row r="40" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G40" s="29"/>
-      <c r="K40" s="30"/>
-      <c r="AG40" s="31"/>
-      <c r="AH40" s="30"/>
-      <c r="AR40" s="31"/>
-      <c r="AS40" s="30"/>
-    </row>
-    <row r="41" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G41" s="29"/>
-      <c r="K41" s="30"/>
-      <c r="AG41" s="31"/>
-      <c r="AH41" s="30"/>
-      <c r="AR41" s="31"/>
-      <c r="AS41" s="30"/>
-    </row>
-    <row r="42" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G42" s="29"/>
-      <c r="K42" s="30"/>
-      <c r="AG42" s="31"/>
-      <c r="AH42" s="30"/>
-      <c r="AR42" s="31"/>
-      <c r="AS42" s="30"/>
-    </row>
-    <row r="43" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K43" s="30"/>
-      <c r="AG43" s="31"/>
-      <c r="AH43" s="30"/>
-      <c r="AR43" s="31"/>
-      <c r="AS43" s="30"/>
-    </row>
-    <row r="44" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K44" s="30"/>
-      <c r="AG44" s="31"/>
-      <c r="AH44" s="30"/>
-      <c r="AR44" s="31"/>
-      <c r="AS44" s="30"/>
-    </row>
-    <row r="45" spans="7:45" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K45" s="30"/>
-      <c r="AG45" s="31"/>
-      <c r="AH45" s="30"/>
-      <c r="AR45" s="31"/>
-      <c r="AS45" s="30"/>
+      <c r="AG16" s="29"/>
+      <c r="AR16" s="29"/>
+    </row>
+    <row r="17" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG17" s="29"/>
+      <c r="AR17" s="29"/>
+    </row>
+    <row r="18" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG18" s="29"/>
+      <c r="AR18" s="29"/>
+    </row>
+    <row r="19" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG19" s="29"/>
+      <c r="AR19" s="29"/>
+    </row>
+    <row r="20" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG20" s="29"/>
+      <c r="AR20" s="29"/>
+    </row>
+    <row r="21" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG21" s="29"/>
+      <c r="AR21" s="29"/>
+    </row>
+    <row r="22" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG22" s="29"/>
+      <c r="AR22" s="29"/>
+    </row>
+    <row r="23" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG23" s="29"/>
+      <c r="AR23" s="29"/>
+    </row>
+    <row r="24" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG24" s="29"/>
+      <c r="AR24" s="29"/>
+    </row>
+    <row r="25" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG25" s="29"/>
+      <c r="AR25" s="29"/>
+    </row>
+    <row r="26" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG26" s="29"/>
+      <c r="AR26" s="29"/>
+    </row>
+    <row r="27" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG27" s="29"/>
+      <c r="AR27" s="29"/>
+    </row>
+    <row r="28" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG28" s="29"/>
+      <c r="AR28" s="29"/>
+    </row>
+    <row r="29" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG29" s="29"/>
+      <c r="AR29" s="29"/>
+    </row>
+    <row r="30" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG30" s="29"/>
+      <c r="AR30" s="29"/>
+    </row>
+    <row r="31" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG31" s="29"/>
+      <c r="AR31" s="29"/>
+    </row>
+    <row r="32" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG32" s="29"/>
+      <c r="AR32" s="29"/>
+    </row>
+    <row r="33" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG33" s="29"/>
+      <c r="AR33" s="29"/>
+    </row>
+    <row r="34" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG34" s="29"/>
+      <c r="AR34" s="29"/>
+    </row>
+    <row r="35" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG35" s="29"/>
+      <c r="AR35" s="29"/>
+    </row>
+    <row r="36" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG36" s="29"/>
+      <c r="AR36" s="29"/>
+    </row>
+    <row r="37" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG37" s="29"/>
+      <c r="AR37" s="29"/>
+    </row>
+    <row r="38" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG38" s="29"/>
+      <c r="AR38" s="29"/>
+    </row>
+    <row r="39" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG39" s="29"/>
+      <c r="AR39" s="29"/>
+    </row>
+    <row r="40" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG40" s="29"/>
+      <c r="AR40" s="29"/>
+    </row>
+    <row r="41" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG41" s="29"/>
+      <c r="AR41" s="29"/>
+    </row>
+    <row r="42" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG42" s="29"/>
+      <c r="AR42" s="29"/>
+    </row>
+    <row r="43" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG43" s="29"/>
+      <c r="AR43" s="29"/>
+    </row>
+    <row r="44" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG44" s="29"/>
+      <c r="AR44" s="29"/>
+    </row>
+    <row r="45" spans="33:44" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG45" s="29"/>
+      <c r="AR45" s="29"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="X7zW4JYrcdpAy7TN45o220MAFZV+CcZVTl5TWLq2/kH1sQ/LQfO8w7BAd41aJo95J/Q72/cAewmpkjf98xW4TA==" saltValue="+km4pe2NPj216RQDX2RkGg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zOvxVl4DIxCdeVOZRivl+k+6eZKcjOjj1Z3r4lcqCPwndzhPL/LcS3ly7FdmuTb30949LOUhuZEytcacwM2hEA==" saltValue="DOdEViT6nyeVjg4Vwmapbw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: SSW-2255 Standard Import Dateien
</commit_message>
<xml_diff>
--- a/Common/Style/Resource/Template/Import_Interessent.xlsx
+++ b/Common/Style/Resource/Template/Import_Interessent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmiezik\Desktop\Schele\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8E4494-C0E1-44A2-89FA-9265384E4F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BA7DAD-DE50-49EB-843F-2EFED73C50C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kl. 1" sheetId="2" r:id="rId1"/>
@@ -5715,7 +5715,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="AO6BhZebrB7pRWRGfiAvVt5mCaD9qOuuat0S+cQeaTax0v55BGfLXrhSGbTg4cH5Sc5Sy9d6AC9fPf7mImS0wg==" saltValue="Vasutm3rels4KXKrP6Y/cA==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0MRvk69Fc+TPRySQgWXv3uWmn8ot1EaVGOL4iW+oW0z/k9koGk8lFCCsmvj4+JRpmb7stcshTg/RX9w1lx1gjA==" saltValue="+AUFqvzqG9HbYCcG4gHwLw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A2:AX2" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>